<commit_message>
updates errors message to be more informative
</commit_message>
<xml_diff>
--- a/data-raw/sherlock-example-outputs/2024/061223_JPE24_E+L_E1-2_P1_SH_RH - NEG-DNA-FAIL.xlsx
+++ b/data-raw/sherlock-example-outputs/2024/061223_JPE24_E+L_E1-2_P1_SH_RH - NEG-DNA-FAIL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanuel\projects\jpe\grunID\data-raw\sherlock-example-outputs\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3725CB2E-848C-40BA-93B8-E2FA816D0C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E10CA8-E0C0-4613-890E-83399CF4FC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3756" yWindow="0" windowWidth="38544" windowHeight="25320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6384" yWindow="1464" windowWidth="35496" windowHeight="22092" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sherlock_output" sheetId="1" r:id="rId1"/>
@@ -1020,7 +1020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AO204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="T92" sqref="T92"/>
     </sheetView>
   </sheetViews>
@@ -6918,7 +6918,7 @@
         <v>2988</v>
       </c>
       <c r="T91" s="13">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="U91" s="13">
         <v>52799</v>
@@ -14327,6 +14327,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B141:B144"/>
+    <mergeCell ref="B145:B148"/>
+    <mergeCell ref="B149:B152"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="B157:B160"/>
     <mergeCell ref="B161:B164"/>
     <mergeCell ref="B189:B192"/>
     <mergeCell ref="B193:B196"/>
@@ -14338,11 +14343,6 @@
     <mergeCell ref="B177:B180"/>
     <mergeCell ref="B181:B184"/>
     <mergeCell ref="B185:B188"/>
-    <mergeCell ref="B141:B144"/>
-    <mergeCell ref="B145:B148"/>
-    <mergeCell ref="B149:B152"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="B157:B160"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14355,7 +14355,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14983,26 +14983,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a5a0c31c-142b-4324-98be-1f22eeaa284f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="114905e2-0299-4464-9b5c-0bcc75829ca8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED9BB87F99202C459DCB42C998E68716" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c08ee5b878ae3ef39f2021558381f3c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5a0c31c-142b-4324-98be-1f22eeaa284f" xmlns:ns3="114905e2-0299-4464-9b5c-0bcc75829ca8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc11d0d83093e52fa8472e404bfcbaef" ns2:_="" ns3:_="">
     <xsd:import namespace="a5a0c31c-142b-4324-98be-1f22eeaa284f"/>
@@ -15237,26 +15217,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1412CB-6D94-4A5C-B7A5-9FB058386B1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a5a0c31c-142b-4324-98be-1f22eeaa284f"/>
-    <ds:schemaRef ds:uri="114905e2-0299-4464-9b5c-0bcc75829ca8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBC3FDB-6B65-4514-8D94-333274499CC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a5a0c31c-142b-4324-98be-1f22eeaa284f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="114905e2-0299-4464-9b5c-0bcc75829ca8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3C8F84-4C33-4311-8670-B3A08FC3537F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15273,4 +15254,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBC3FDB-6B65-4514-8D94-333274499CC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1412CB-6D94-4A5C-B7A5-9FB058386B1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a5a0c31c-142b-4324-98be-1f22eeaa284f"/>
+    <ds:schemaRef ds:uri="114905e2-0299-4464-9b5c-0bcc75829ca8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>